<commit_message>
Creating function for orders
</commit_message>
<xml_diff>
--- a/db/persons_data.xlsx
+++ b/db/persons_data.xlsx
@@ -518,7 +518,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1000000</v>
+        <v>1008000</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>100000</v>
+        <v>115700</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>

</xml_diff>